<commit_message>
Update optimization jan 2024 to aug 2025 -gbpusd and eurusd-1h.xlsx
</commit_message>
<xml_diff>
--- a/OPTIMIZATION/optimization jan 2024 to aug 2025 -gbpusd and eurusd-1h.xlsx
+++ b/OPTIMIZATION/optimization jan 2024 to aug 2025 -gbpusd and eurusd-1h.xlsx
@@ -8,22 +8,48 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\BOTS\REHOBOAM\OPTIMIZATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AC04A6-9148-484E-B90F-03B2B4496699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46AF8BB-47E3-4C9F-B1BC-18750132CB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{2112105C-1B99-4D4F-85A4-5682E24BD8D2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{2112105C-1B99-4D4F-85A4-5682E24BD8D2}"/>
   </bookViews>
   <sheets>
     <sheet name="PREDICTOR" sheetId="4" r:id="rId1"/>
     <sheet name="Tester Optimizator Results" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">PREDICTOR!$B$26:$B$27</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">PREDICTOR!$B$28</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'Tester Optimizator Results'!#REF!</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -780,7 +806,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -796,12 +822,11 @@
     <xf numFmtId="2" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -852,17 +877,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -885,21 +900,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1235,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D3A376-5C30-45C0-8A76-1B2BAD76ABFC}">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,48 +1272,48 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
         <v>0.2585173770811891</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5">
         <v>6.683123425293773E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>3.3973179120998918E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>5413.3769607743543</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>148</v>
       </c>
     </row>
@@ -1308,272 +1323,270 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
         <v>5</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12">
         <v>298019150.70274067</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12">
         <v>59603830.140548132</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12">
         <v>2.0339376139148353</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12">
         <v>7.7395373962280301E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13">
         <v>142</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13">
         <v>4161260316.9608469</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13">
         <v>29304650.119442582</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>147</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>4459279467.6635876</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17">
         <v>-1747.5042403536625</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17">
         <v>1929.223133204943</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17">
         <v>-0.90580721860337743</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17">
         <v>0.3665722893580392</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17">
         <v>-5561.2137392440209</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17">
         <v>2066.2052585366964</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17">
         <v>-5561.2137392440209</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17">
         <v>2066.2052585366964</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18">
         <v>1886.9718673468146</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18">
         <v>1183.4309246223781</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18">
         <v>1.5944926130343686</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18">
         <v>0.11304910383526086</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18">
         <v>-452.44739465180055</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18">
         <v>4226.3911293454294</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18">
         <v>-452.44739465180055</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18">
         <v>4226.3911293454294</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19">
         <v>4155.5956874526391</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19">
         <v>2181.7269398833596</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19">
         <v>1.904727677641826</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19">
         <v>5.8837602271058102E-2</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19">
         <v>-157.2661124137594</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19">
         <v>8468.4574873190377</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19">
         <v>-157.2661124137594</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19">
         <v>8468.4574873190377</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20">
         <v>-439.75003891519623</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20">
         <v>216.89429973812076</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>-2.0274854592589691</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20">
         <v>4.4483556194091528E-2</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>-868.50907509381364</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20">
         <v>-10.991002736578821</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20">
         <v>-868.50907509381364</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20">
         <v>-10.991002736578821</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21">
         <v>-1026.6474885853411</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21">
         <v>669.59847197626073</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21">
         <v>-1.5332285415097824</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>0.12744451890216346</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>-2350.3171093077763</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21">
         <v>297.02213213709433</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21">
         <v>-2350.3171093077763</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21">
         <v>297.02213213709433</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>-104.37110559978575</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>340.36149674638233</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>-0.30664780416557236</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>0.75956065138194939</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>-777.20145417736853</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>568.45924297779698</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="9">
         <v>-777.20145417736853</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="9">
         <v>568.45924297779698</v>
       </c>
     </row>
@@ -1587,7 +1600,7 @@
         <v>48</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1.9168918425164101</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1595,16 +1608,16 @@
         <v>49</v>
       </c>
       <c r="B27">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="14" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
+        <v>1.9264274665800236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="13" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <f>B17+(B18*B26)+(B19*B27)+(B20*B26*B26)+(B21*B27*B27)+(B22*B26*B27)</f>
-        <v>3269.7127616786984</v>
+        <v>4063.7885699801864</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1639,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>$B$17+($B$18*B32)+($B$19*C32)+($B$20*B32*B32)+($B$21*C32*C32)+($B$22*B32*C32)</f>
+        <f t="shared" ref="A32:A63" si="0">$B$17+($B$18*B32)+($B$19*C32)+($B$20*B32*B32)+($B$21*C32*C32)+($B$22*B32*C32)</f>
         <v>4062.8993482731344</v>
       </c>
       <c r="B32">
@@ -1638,7 +1651,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>$B$17+($B$18*B33)+($B$19*C33)+($B$20*B33*B33)+($B$21*C33*C33)+($B$22*B33*C33)</f>
+        <f t="shared" si="0"/>
         <v>4054.5563368439543</v>
       </c>
       <c r="B33">
@@ -1650,7 +1663,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>$B$17+($B$18*B34)+($B$19*C34)+($B$20*B34*B34)+($B$21*C34*C34)+($B$22*B34*C34)</f>
+        <f t="shared" si="0"/>
         <v>4039.8269870403083</v>
       </c>
       <c r="B34">
@@ -1662,7 +1675,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>$B$17+($B$18*B35)+($B$19*C35)+($B$20*B35*B35)+($B$21*C35*C35)+($B$22*B35*C35)</f>
+        <f t="shared" si="0"/>
         <v>4014.7979527527655</v>
       </c>
       <c r="B35">
@@ -1674,7 +1687,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>$B$17+($B$18*B36)+($B$19*C36)+($B$20*B36*B36)+($B$21*C36*C36)+($B$22*B36*C36)</f>
+        <f t="shared" si="0"/>
         <v>3985.3392531454751</v>
       </c>
       <c r="B36">
@@ -1686,7 +1699,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>$B$17+($B$18*B37)+($B$19*C37)+($B$20*B37*B37)+($B$21*C37*C37)+($B$22*B37*C37)</f>
+        <f t="shared" si="0"/>
         <v>3943.6241959995723</v>
       </c>
       <c r="B37">
@@ -1698,7 +1711,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>$B$17+($B$18*B38)+($B$19*C38)+($B$20*B38*B38)+($B$21*C38*C38)+($B$22*B38*C38)</f>
+        <f t="shared" si="0"/>
         <v>3899.4361465886368</v>
       </c>
       <c r="B38">
@@ -1710,7 +1723,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>$B$17+($B$18*B39)+($B$19*C39)+($B$20*B39*B39)+($B$21*C39*C39)+($B$22*B39*C39)</f>
+        <f t="shared" si="0"/>
         <v>3841.0350665843703</v>
       </c>
       <c r="B39">
@@ -1722,7 +1735,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>$B$17+($B$18*B40)+($B$19*C40)+($B$20*B40*B40)+($B$21*C40*C40)+($B$22*B40*C40)</f>
+        <f t="shared" si="0"/>
         <v>3782.1176673697923</v>
       </c>
       <c r="B40">
@@ -1734,7 +1747,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>$B$17+($B$18*B41)+($B$19*C41)+($B$20*B41*B41)+($B$21*C41*C41)+($B$22*B41*C41)</f>
+        <f t="shared" si="0"/>
         <v>3707.0305645071639</v>
       </c>
       <c r="B41">
@@ -1746,7 +1759,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>$B$17+($B$18*B42)+($B$19*C42)+($B$20*B42*B42)+($B$21*C42*C42)+($B$22*B42*C42)</f>
+        <f t="shared" si="0"/>
         <v>3633.3838154889386</v>
       </c>
       <c r="B42">
@@ -1758,7 +1771,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>$B$17+($B$18*B43)+($B$19*C43)+($B$20*B43*B43)+($B$21*C43*C43)+($B$22*B43*C43)</f>
+        <f t="shared" si="0"/>
         <v>3541.6106897679515</v>
       </c>
       <c r="B43">
@@ -1770,7 +1783,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f>$B$17+($B$18*B44)+($B$19*C44)+($B$20*B44*B44)+($B$21*C44*C44)+($B$22*B44*C44)</f>
+        <f t="shared" si="0"/>
         <v>3453.2345909460819</v>
       </c>
       <c r="B44">
@@ -1782,7 +1795,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f>$B$17+($B$18*B45)+($B$19*C45)+($B$20*B45*B45)+($B$21*C45*C45)+($B$22*B45*C45)</f>
+        <f t="shared" si="0"/>
         <v>3344.7754423667325</v>
       </c>
       <c r="B45">
@@ -1794,7 +1807,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f>$B$17+($B$18*B46)+($B$19*C46)+($B$20*B46*B46)+($B$21*C46*C46)+($B$22*B46*C46)</f>
+        <f t="shared" si="0"/>
         <v>3241.6699937412168</v>
       </c>
       <c r="B46">
@@ -1806,7 +1819,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f>$B$17+($B$18*B47)+($B$19*C47)+($B$20*B47*B47)+($B$21*C47*C47)+($B$22*B47*C47)</f>
+        <f t="shared" si="0"/>
         <v>3116.5248223035069</v>
       </c>
       <c r="B47">
@@ -1818,7 +1831,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f>$B$17+($B$18*B48)+($B$19*C48)+($B$20*B48*B48)+($B$21*C48*C48)+($B$22*B48*C48)</f>
+        <f t="shared" si="0"/>
         <v>2998.690023874346</v>
       </c>
       <c r="B48">
@@ -1830,7 +1843,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f>$B$17+($B$18*B49)+($B$19*C49)+($B$20*B49*B49)+($B$21*C49*C49)+($B$22*B49*C49)</f>
+        <f t="shared" si="0"/>
         <v>2856.8588295782752</v>
       </c>
       <c r="B49">
@@ -1842,7 +1855,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f>$B$17+($B$18*B50)+($B$19*C50)+($B$20*B50*B50)+($B$21*C50*C50)+($B$22*B50*C50)</f>
+        <f t="shared" si="0"/>
         <v>2724.2946813454682</v>
       </c>
       <c r="B50">
@@ -1854,7 +1867,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f>$B$17+($B$18*B51)+($B$19*C51)+($B$20*B51*B51)+($B$21*C51*C51)+($B$22*B51*C51)</f>
+        <f t="shared" si="0"/>
         <v>2565.7774641910364</v>
       </c>
       <c r="B51">
@@ -1866,7 +1879,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f>$B$17+($B$18*B52)+($B$19*C52)+($B$20*B52*B52)+($B$21*C52*C52)+($B$22*B52*C52)</f>
+        <f t="shared" si="0"/>
         <v>2418.4839661545848</v>
       </c>
       <c r="B52">
@@ -1878,7 +1891,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f>$B$17+($B$18*B53)+($B$19*C53)+($B$20*B53*B53)+($B$21*C53*C53)+($B$22*B53*C53)</f>
+        <f t="shared" si="0"/>
         <v>2243.280726141792</v>
       </c>
       <c r="B53">
@@ -1890,7 +1903,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f>$B$17+($B$18*B54)+($B$19*C54)+($B$20*B54*B54)+($B$21*C54*C54)+($B$22*B54*C54)</f>
+        <f t="shared" si="0"/>
         <v>2081.2578783016938</v>
       </c>
       <c r="B54">
@@ -1902,7 +1915,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f>$B$17+($B$18*B55)+($B$19*C55)+($B$20*B55*B55)+($B$21*C55*C55)+($B$22*B55*C55)</f>
+        <f t="shared" si="0"/>
         <v>1889.3686154305378</v>
       </c>
       <c r="B55">
@@ -1914,7 +1927,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f>$B$17+($B$18*B56)+($B$19*C56)+($B$20*B56*B56)+($B$21*C56*C56)+($B$22*B56*C56)</f>
+        <f t="shared" si="0"/>
         <v>1712.6164177867965</v>
       </c>
       <c r="B56">
@@ -1926,7 +1939,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f>$B$17+($B$18*B57)+($B$19*C57)+($B$20*B57*B57)+($B$21*C57*C57)+($B$22*B57*C57)</f>
+        <f t="shared" si="0"/>
         <v>1504.0411320572796</v>
       </c>
       <c r="B57">
@@ -1938,7 +1951,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f>$B$17+($B$18*B58)+($B$19*C58)+($B$20*B58*B58)+($B$21*C58*C58)+($B$22*B58*C58)</f>
+        <f t="shared" si="0"/>
         <v>1312.5595846098934</v>
       </c>
       <c r="B58">
@@ -1950,7 +1963,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f>$B$17+($B$18*B59)+($B$19*C59)+($B$20*B59*B59)+($B$21*C59*C59)+($B$22*B59*C59)</f>
+        <f t="shared" si="0"/>
         <v>1087.2982760220154</v>
       </c>
       <c r="B59">
@@ -1962,7 +1975,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f>$B$17+($B$18*B60)+($B$19*C60)+($B$20*B60*B60)+($B$21*C60*C60)+($B$22*B60*C60)</f>
+        <f t="shared" si="0"/>
         <v>881.08737877098361</v>
       </c>
       <c r="B60">
@@ -1974,7 +1987,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f>$B$17+($B$18*B61)+($B$19*C61)+($B$20*B61*B61)+($B$21*C61*C61)+($B$22*B61*C61)</f>
+        <f t="shared" si="0"/>
         <v>639.14004732474496</v>
       </c>
       <c r="B61">
@@ -1986,7 +1999,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f>$B$17+($B$18*B62)+($B$19*C62)+($B$20*B62*B62)+($B$21*C62*C62)+($B$22*B62*C62)</f>
+        <f t="shared" si="0"/>
         <v>418.19980027006756</v>
       </c>
       <c r="B62">
@@ -1998,7 +2011,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f>$B$17+($B$18*B63)+($B$19*C63)+($B$20*B63*B63)+($B$21*C63*C63)+($B$22*B63*C63)</f>
+        <f t="shared" si="0"/>
         <v>159.56644596546812</v>
       </c>
       <c r="B63">
@@ -2010,7 +2023,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f>$B$17+($B$18*B64)+($B$19*C64)+($B$20*B64*B64)+($B$21*C64*C64)+($B$22*B64*C64)</f>
+        <f t="shared" ref="A64:A95" si="1">$B$17+($B$18*B64)+($B$19*C64)+($B$20*B64*B64)+($B$21*C64*C64)+($B$22*B64*C64)</f>
         <v>-76.103150892855567</v>
       </c>
       <c r="B64">
@@ -2022,7 +2035,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f>$B$17+($B$18*B65)+($B$19*C65)+($B$20*B65*B65)+($B$21*C65*C65)+($B$22*B65*C65)</f>
+        <f t="shared" si="1"/>
         <v>-351.42252805581643</v>
       </c>
       <c r="B65">
@@ -2034,7 +2047,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f>$B$17+($B$18*B66)+($B$19*C66)+($B$20*B66*B66)+($B$21*C66*C66)+($B$22*B66*C66)</f>
+        <f t="shared" si="1"/>
         <v>-601.82147471778444</v>
       </c>
       <c r="B66">
@@ -2046,7 +2059,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f>$B$17+($B$18*B67)+($B$19*C67)+($B$20*B67*B67)+($B$21*C67*C67)+($B$22*B67*C67)</f>
+        <f t="shared" si="1"/>
         <v>-893.82687473910732</v>
       </c>
       <c r="B67">
@@ -2058,7 +2071,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f>$B$17+($B$18*B68)+($B$19*C68)+($B$20*B68*B68)+($B$21*C68*C68)+($B$22*B68*C68)</f>
+        <f t="shared" si="1"/>
         <v>-1158.95517120472</v>
       </c>
       <c r="B68">
@@ -2070,7 +2083,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f>$B$17+($B$18*B69)+($B$19*C69)+($B$20*B69*B69)+($B$21*C69*C69)+($B$22*B69*C69)</f>
+        <f t="shared" si="1"/>
         <v>-1467.6465940844023</v>
       </c>
       <c r="B69">
@@ -2082,7 +2095,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f>$B$17+($B$18*B70)+($B$19*C70)+($B$20*B70*B70)+($B$21*C70*C70)+($B$22*B70*C70)</f>
+        <f t="shared" si="1"/>
         <v>-1747.5042403536625</v>
       </c>
       <c r="B70">
@@ -2094,7 +2107,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f>$B$17+($B$18*B71)+($B$19*C71)+($B$20*B71*B71)+($B$21*C71*C71)+($B$22*B71*C71)</f>
+        <f t="shared" si="1"/>
         <v>-2072.8816860917073</v>
       </c>
       <c r="B71">
@@ -2106,7 +2119,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f>$B$17+($B$18*B72)+($B$19*C72)+($B$20*B72*B72)+($B$21*C72*C72)+($B$22*B72*C72)</f>
+        <f t="shared" si="1"/>
         <v>-2709.5321507610165</v>
       </c>
       <c r="B72">
@@ -2118,7 +2131,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f>$B$17+($B$18*B73)+($B$19*C73)+($B$20*B73*B73)+($B$21*C73*C73)+($B$22*B73*C73)</f>
+        <f t="shared" si="1"/>
         <v>-3377.5979880923314</v>
       </c>
       <c r="B73">
@@ -2130,7 +2143,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f>$B$17+($B$18*B74)+($B$19*C74)+($B$20*B74*B74)+($B$21*C74*C74)+($B$22*B74*C74)</f>
+        <f t="shared" si="1"/>
         <v>-4077.0791980856534</v>
       </c>
       <c r="B74">
@@ -2142,7 +2155,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f>$B$17+($B$18*B75)+($B$19*C75)+($B$20*B75*B75)+($B$21*C75*C75)+($B$22*B75*C75)</f>
+        <f t="shared" si="1"/>
         <v>-4807.9757807409842</v>
       </c>
       <c r="B75">
@@ -2154,7 +2167,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f>$B$17+($B$18*B76)+($B$19*C76)+($B$20*B76*B76)+($B$21*C76*C76)+($B$22*B76*C76)</f>
+        <f t="shared" si="1"/>
         <v>-5570.2877360583225</v>
       </c>
       <c r="B76">
@@ -2166,7 +2179,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f>$B$17+($B$18*B77)+($B$19*C77)+($B$20*B77*B77)+($B$21*C77*C77)+($B$22*B77*C77)</f>
+        <f t="shared" si="1"/>
         <v>-6364.0150640376605</v>
       </c>
       <c r="B77">
@@ -2178,7 +2191,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f>$B$17+($B$18*B78)+($B$19*C78)+($B$20*B78*B78)+($B$21*C78*C78)+($B$22*B78*C78)</f>
+        <f t="shared" si="1"/>
         <v>-7189.157764679012</v>
       </c>
       <c r="B78">
@@ -2190,7 +2203,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f>$B$17+($B$18*B79)+($B$19*C79)+($B$20*B79*B79)+($B$21*C79*C79)+($B$22*B79*C79)</f>
+        <f t="shared" si="1"/>
         <v>-8045.7158379823732</v>
       </c>
       <c r="B79">
@@ -2202,7 +2215,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f>$B$17+($B$18*B80)+($B$19*C80)+($B$20*B80*B80)+($B$21*C80*C80)+($B$22*B80*C80)</f>
+        <f t="shared" si="1"/>
         <v>-8933.6892839477259</v>
       </c>
       <c r="B80">
@@ -2214,7 +2227,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f>$B$17+($B$18*B81)+($B$19*C81)+($B$20*B81*B81)+($B$21*C81*C81)+($B$22*B81*C81)</f>
+        <f t="shared" si="1"/>
         <v>-9853.0781025751003</v>
       </c>
       <c r="B81">
@@ -2226,7 +2239,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f>$B$17+($B$18*B82)+($B$19*C82)+($B$20*B82*B82)+($B$21*C82*C82)+($B$22*B82*C82)</f>
+        <f t="shared" si="1"/>
         <v>-10803.882293864472</v>
       </c>
       <c r="B82">
@@ -2238,7 +2251,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f>$B$17+($B$18*B83)+($B$19*C83)+($B$20*B83*B83)+($B$21*C83*C83)+($B$22*B83*C83)</f>
+        <f t="shared" si="1"/>
         <v>-11786.101857815847</v>
       </c>
       <c r="B83">
@@ -2250,7 +2263,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f>$B$17+($B$18*B84)+($B$19*C84)+($B$20*B84*B84)+($B$21*C84*C84)+($B$22*B84*C84)</f>
+        <f t="shared" si="1"/>
         <v>-12799.73679442924</v>
       </c>
       <c r="B84">
@@ -2262,7 +2275,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f>$B$17+($B$18*B85)+($B$19*C85)+($B$20*B85*B85)+($B$21*C85*C85)+($B$22*B85*C85)</f>
+        <f t="shared" si="1"/>
         <v>-13844.787103704633</v>
       </c>
       <c r="B85">
@@ -2274,7 +2287,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f>$B$17+($B$18*B86)+($B$19*C86)+($B$20*B86*B86)+($B$21*C86*C86)+($B$22*B86*C86)</f>
+        <f t="shared" si="1"/>
         <v>-14921.252785642035</v>
       </c>
       <c r="B86">
@@ -2286,7 +2299,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f>$B$17+($B$18*B87)+($B$19*C87)+($B$20*B87*B87)+($B$21*C87*C87)+($B$22*B87*C87)</f>
+        <f t="shared" si="1"/>
         <v>-16029.13384024144</v>
       </c>
       <c r="B87">
@@ -2298,7 +2311,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f>$B$17+($B$18*B88)+($B$19*C88)+($B$20*B88*B88)+($B$21*C88*C88)+($B$22*B88*C88)</f>
+        <f t="shared" si="1"/>
         <v>-17168.430267502845</v>
       </c>
       <c r="B88">
@@ -2310,7 +2323,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <f>$B$17+($B$18*B89)+($B$19*C89)+($B$20*B89*B89)+($B$21*C89*C89)+($B$22*B89*C89)</f>
+        <f t="shared" si="1"/>
         <v>-18339.142067426274</v>
       </c>
       <c r="B89">
@@ -2322,7 +2335,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <f>$B$17+($B$18*B90)+($B$19*C90)+($B$20*B90*B90)+($B$21*C90*C90)+($B$22*B90*C90)</f>
+        <f t="shared" si="1"/>
         <v>-19541.269240011694</v>
       </c>
       <c r="B90">
@@ -2334,7 +2347,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <f>$B$17+($B$18*B91)+($B$19*C91)+($B$20*B91*B91)+($B$21*C91*C91)+($B$22*B91*C91)</f>
+        <f t="shared" si="1"/>
         <v>-20774.811785259142</v>
       </c>
       <c r="B91">
@@ -2346,7 +2359,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <f>$B$17+($B$18*B92)+($B$19*C92)+($B$20*B92*B92)+($B$21*C92*C92)+($B$22*B92*C92)</f>
+        <f t="shared" si="1"/>
         <v>-22039.769703168568</v>
       </c>
       <c r="B92">
@@ -2358,7 +2371,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <f>$B$17+($B$18*B93)+($B$19*C93)+($B$20*B93*B93)+($B$21*C93*C93)+($B$22*B93*C93)</f>
+        <f t="shared" si="1"/>
         <v>-23336.14299374001</v>
       </c>
       <c r="B93">
@@ -2370,7 +2383,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f>$B$17+($B$18*B94)+($B$19*C94)+($B$20*B94*B94)+($B$21*C94*C94)+($B$22*B94*C94)</f>
+        <f t="shared" si="1"/>
         <v>-24663.931656973469</v>
       </c>
       <c r="B94">
@@ -2382,7 +2395,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <f>$B$17+($B$18*B95)+($B$19*C95)+($B$20*B95*B95)+($B$21*C95*C95)+($B$22*B95*C95)</f>
+        <f t="shared" si="1"/>
         <v>-26023.135692868924</v>
       </c>
       <c r="B95">
@@ -2394,7 +2407,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <f>$B$17+($B$18*B96)+($B$19*C96)+($B$20*B96*B96)+($B$21*C96*C96)+($B$22*B96*C96)</f>
+        <f t="shared" ref="A96:A127" si="2">$B$17+($B$18*B96)+($B$19*C96)+($B$20*B96*B96)+($B$21*C96*C96)+($B$22*B96*C96)</f>
         <v>-27413.755101426399</v>
       </c>
       <c r="B96">
@@ -2406,7 +2419,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f>$B$17+($B$18*B97)+($B$19*C97)+($B$20*B97*B97)+($B$21*C97*C97)+($B$22*B97*C97)</f>
+        <f t="shared" si="2"/>
         <v>-28835.789882645859</v>
       </c>
       <c r="B97">
@@ -2418,7 +2431,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <f>$B$17+($B$18*B98)+($B$19*C98)+($B$20*B98*B98)+($B$21*C98*C98)+($B$22*B98*C98)</f>
+        <f t="shared" si="2"/>
         <v>-30289.240036527335</v>
       </c>
       <c r="B98">
@@ -2430,7 +2443,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <f>$B$17+($B$18*B99)+($B$19*C99)+($B$20*B99*B99)+($B$21*C99*C99)+($B$22*B99*C99)</f>
+        <f t="shared" si="2"/>
         <v>-31774.105563070825</v>
       </c>
       <c r="B99">
@@ -2442,7 +2455,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f>$B$17+($B$18*B100)+($B$19*C100)+($B$20*B100*B100)+($B$21*C100*C100)+($B$22*B100*C100)</f>
+        <f t="shared" si="2"/>
         <v>-33290.386462276314</v>
       </c>
       <c r="B100">
@@ -2454,7 +2467,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f>$B$17+($B$18*B101)+($B$19*C101)+($B$20*B101*B101)+($B$21*C101*C101)+($B$22*B101*C101)</f>
+        <f t="shared" si="2"/>
         <v>-34838.08273414382</v>
       </c>
       <c r="B101">
@@ -2466,7 +2479,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f>$B$17+($B$18*B102)+($B$19*C102)+($B$20*B102*B102)+($B$21*C102*C102)+($B$22*B102*C102)</f>
+        <f t="shared" si="2"/>
         <v>-36417.194378673317</v>
       </c>
       <c r="B102">
@@ -2478,7 +2491,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <f>$B$17+($B$18*B103)+($B$19*C103)+($B$20*B103*B103)+($B$21*C103*C103)+($B$22*B103*C103)</f>
+        <f t="shared" si="2"/>
         <v>-38027.721395864821</v>
       </c>
       <c r="B103">
@@ -2490,7 +2503,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <f>$B$17+($B$18*B104)+($B$19*C104)+($B$20*B104*B104)+($B$21*C104*C104)+($B$22*B104*C104)</f>
+        <f t="shared" si="2"/>
         <v>-39669.663785718338</v>
       </c>
       <c r="B104">
@@ -2502,7 +2515,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <f>$B$17+($B$18*B105)+($B$19*C105)+($B$20*B105*B105)+($B$21*C105*C105)+($B$22*B105*C105)</f>
+        <f t="shared" si="2"/>
         <v>-41343.021548233868</v>
       </c>
       <c r="B105">
@@ -2514,7 +2527,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <f>$B$17+($B$18*B106)+($B$19*C106)+($B$20*B106*B106)+($B$21*C106*C106)+($B$22*B106*C106)</f>
+        <f t="shared" si="2"/>
         <v>-43047.794683411397</v>
       </c>
       <c r="B106">
@@ -2526,7 +2539,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <f>$B$17+($B$18*B107)+($B$19*C107)+($B$20*B107*B107)+($B$21*C107*C107)+($B$22*B107*C107)</f>
+        <f t="shared" si="2"/>
         <v>-44783.983191250933</v>
       </c>
       <c r="B107">
@@ -2538,7 +2551,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <f>$B$17+($B$18*B108)+($B$19*C108)+($B$20*B108*B108)+($B$21*C108*C108)+($B$22*B108*C108)</f>
+        <f t="shared" si="2"/>
         <v>-46551.587071752474</v>
       </c>
       <c r="B108">
@@ -2550,7 +2563,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <f>$B$17+($B$18*B109)+($B$19*C109)+($B$20*B109*B109)+($B$21*C109*C109)+($B$22*B109*C109)</f>
+        <f t="shared" si="2"/>
         <v>-48350.606324916022</v>
       </c>
       <c r="B109">
@@ -2562,7 +2575,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <f>$B$17+($B$18*B110)+($B$19*C110)+($B$20*B110*B110)+($B$21*C110*C110)+($B$22*B110*C110)</f>
+        <f t="shared" si="2"/>
         <v>-50181.040950741575</v>
       </c>
       <c r="B110">
@@ -2574,7 +2587,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <f>$B$17+($B$18*B111)+($B$19*C111)+($B$20*B111*B111)+($B$21*C111*C111)+($B$22*B111*C111)</f>
+        <f t="shared" si="2"/>
         <v>-52042.89094922915</v>
       </c>
       <c r="B111">
@@ -2586,7 +2599,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <f>$B$17+($B$18*B112)+($B$19*C112)+($B$20*B112*B112)+($B$21*C112*C112)+($B$22*B112*C112)</f>
+        <f t="shared" si="2"/>
         <v>-53936.156320378708</v>
       </c>
       <c r="B112">
@@ -2598,7 +2611,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <f>$B$17+($B$18*B113)+($B$19*C113)+($B$20*B113*B113)+($B$21*C113*C113)+($B$22*B113*C113)</f>
+        <f t="shared" si="2"/>
         <v>-55860.837064190258</v>
       </c>
       <c r="B113">
@@ -2610,7 +2623,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
-        <f>$B$17+($B$18*B114)+($B$19*C114)+($B$20*B114*B114)+($B$21*C114*C114)+($B$22*B114*C114)</f>
+        <f t="shared" si="2"/>
         <v>-57816.933180663851</v>
       </c>
       <c r="B114">
@@ -2622,7 +2635,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <f>$B$17+($B$18*B115)+($B$19*C115)+($B$20*B115*B115)+($B$21*C115*C115)+($B$22*B115*C115)</f>
+        <f t="shared" si="2"/>
         <v>-59804.444669799457</v>
       </c>
       <c r="B115">
@@ -2634,7 +2647,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
-        <f>$B$17+($B$18*B116)+($B$19*C116)+($B$20*B116*B116)+($B$21*C116*C116)+($B$22*B116*C116)</f>
+        <f t="shared" si="2"/>
         <v>-61823.37153159704</v>
       </c>
       <c r="B116">
@@ -2646,7 +2659,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <f>$B$17+($B$18*B117)+($B$19*C117)+($B$20*B117*B117)+($B$21*C117*C117)+($B$22*B117*C117)</f>
+        <f t="shared" si="2"/>
         <v>-63873.713766056651</v>
       </c>
       <c r="B117">
@@ -2658,7 +2671,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
-        <f>$B$17+($B$18*B118)+($B$19*C118)+($B$20*B118*B118)+($B$21*C118*C118)+($B$22*B118*C118)</f>
+        <f t="shared" si="2"/>
         <v>-65955.471373178254</v>
       </c>
       <c r="B118">
@@ -2670,7 +2683,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
-        <f>$B$17+($B$18*B119)+($B$19*C119)+($B$20*B119*B119)+($B$21*C119*C119)+($B$22*B119*C119)</f>
+        <f t="shared" si="2"/>
         <v>-68068.644352961841</v>
       </c>
       <c r="B119">
@@ -2682,7 +2695,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
-        <f>$B$17+($B$18*B120)+($B$19*C120)+($B$20*B120*B120)+($B$21*C120*C120)+($B$22*B120*C120)</f>
+        <f t="shared" si="2"/>
         <v>-70213.232705407499</v>
       </c>
       <c r="B120">
@@ -2694,7 +2707,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
-        <f>$B$17+($B$18*B121)+($B$19*C121)+($B$20*B121*B121)+($B$21*C121*C121)+($B$22*B121*C121)</f>
+        <f t="shared" si="2"/>
         <v>-72389.236430515128</v>
       </c>
       <c r="B121">
@@ -2706,7 +2719,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
-        <f>$B$17+($B$18*B122)+($B$19*C122)+($B$20*B122*B122)+($B$21*C122*C122)+($B$22*B122*C122)</f>
+        <f t="shared" si="2"/>
         <v>-74596.65552828474</v>
       </c>
       <c r="B122">
@@ -2718,7 +2731,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
-        <f>$B$17+($B$18*B123)+($B$19*C123)+($B$20*B123*B123)+($B$21*C123*C123)+($B$22*B123*C123)</f>
+        <f t="shared" si="2"/>
         <v>-76835.489998716395</v>
       </c>
       <c r="B123">
@@ -2730,7 +2743,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
-        <f>$B$17+($B$18*B124)+($B$19*C124)+($B$20*B124*B124)+($B$21*C124*C124)+($B$22*B124*C124)</f>
+        <f t="shared" si="2"/>
         <v>-79105.73984181002</v>
       </c>
       <c r="B124">
@@ -2742,7 +2755,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
-        <f>$B$17+($B$18*B125)+($B$19*C125)+($B$20*B125*B125)+($B$21*C125*C125)+($B$22*B125*C125)</f>
+        <f t="shared" si="2"/>
         <v>-81407.405057565687</v>
       </c>
       <c r="B125">
@@ -2754,7 +2767,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
-        <f>$B$17+($B$18*B126)+($B$19*C126)+($B$20*B126*B126)+($B$21*C126*C126)+($B$22*B126*C126)</f>
+        <f t="shared" si="2"/>
         <v>-83740.485645983368</v>
       </c>
       <c r="B126">
@@ -2766,7 +2779,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
-        <f>$B$17+($B$18*B127)+($B$19*C127)+($B$20*B127*B127)+($B$21*C127*C127)+($B$22*B127*C127)</f>
+        <f t="shared" si="2"/>
         <v>-86104.981607063019</v>
       </c>
       <c r="B127">
@@ -2778,7 +2791,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
-        <f>$B$17+($B$18*B128)+($B$19*C128)+($B$20*B128*B128)+($B$21*C128*C128)+($B$22*B128*C128)</f>
+        <f t="shared" ref="A128:A159" si="3">$B$17+($B$18*B128)+($B$19*C128)+($B$20*B128*B128)+($B$21*C128*C128)+($B$22*B128*C128)</f>
         <v>-88500.892940804668</v>
       </c>
       <c r="B128">
@@ -2790,7 +2803,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
-        <f>$B$17+($B$18*B129)+($B$19*C129)+($B$20*B129*B129)+($B$21*C129*C129)+($B$22*B129*C129)</f>
+        <f t="shared" si="3"/>
         <v>-90928.219647208345</v>
       </c>
       <c r="B129">
@@ -2802,7 +2815,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
-        <f>$B$17+($B$18*B130)+($B$19*C130)+($B$20*B130*B130)+($B$21*C130*C130)+($B$22*B130*C130)</f>
+        <f t="shared" si="3"/>
         <v>-93386.96172627405</v>
       </c>
       <c r="B130">
@@ -2814,7 +2827,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
-        <f>$B$17+($B$18*B131)+($B$19*C131)+($B$20*B131*B131)+($B$21*C131*C131)+($B$22*B131*C131)</f>
+        <f t="shared" si="3"/>
         <v>-95877.119178001725</v>
       </c>
       <c r="B131">
@@ -2826,7 +2839,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
-        <f>$B$17+($B$18*B132)+($B$19*C132)+($B$20*B132*B132)+($B$21*C132*C132)+($B$22*B132*C132)</f>
+        <f t="shared" si="3"/>
         <v>-98398.692002391443</v>
       </c>
       <c r="B132">
@@ -2841,10 +2854,10 @@
     <sortCondition descending="1" ref="A32:A132"/>
   </sortState>
   <conditionalFormatting sqref="A32:A132">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2856,7 +2869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E0279F-C843-49B4-9FCB-9E222CFD0814}">
   <dimension ref="A1:S149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
@@ -12264,34 +12277,22 @@
     <sortCondition descending="1" ref="L2:L149"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33E6FF2-511A-4EA1-B6B3-5E55BE485ABD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update on best settings
</commit_message>
<xml_diff>
--- a/OPTIMIZATION/optimization jan 2024 to aug 2025 -gbpusd and eurusd-1h.xlsx
+++ b/OPTIMIZATION/optimization jan 2024 to aug 2025 -gbpusd and eurusd-1h.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\BOTS\REHOBOAM\OPTIMIZATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46AF8BB-47E3-4C9F-B1BC-18750132CB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA33DCBB-2990-4826-9A26-7E32329416F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{2112105C-1B99-4D4F-85A4-5682E24BD8D2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{2112105C-1B99-4D4F-85A4-5682E24BD8D2}"/>
   </bookViews>
   <sheets>
     <sheet name="PREDICTOR" sheetId="4" r:id="rId1"/>
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D3A376-5C30-45C0-8A76-1B2BAD76ABFC}">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,7 +1600,7 @@
         <v>48</v>
       </c>
       <c r="B26">
-        <v>1.9168918425164101</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1608,7 +1608,7 @@
         <v>49</v>
       </c>
       <c r="B27">
-        <v>1.9264274665800236</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="13" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B28" s="14">
         <f>B17+(B18*B26)+(B19*B27)+(B20*B26*B26)+(B21*B27*B27)+(B22*B26*B27)</f>
-        <v>4063.7885699801864</v>
+        <v>-145.5055119334404</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
-        <f t="shared" ref="A128:A159" si="3">$B$17+($B$18*B128)+($B$19*C128)+($B$20*B128*B128)+($B$21*C128*C128)+($B$22*B128*C128)</f>
+        <f t="shared" ref="A128:A132" si="3">$B$17+($B$18*B128)+($B$19*C128)+($B$20*B128*B128)+($B$21*C128*C128)+($B$22*B128*C128)</f>
         <v>-88500.892940804668</v>
       </c>
       <c r="B128">
@@ -2869,7 +2869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E0279F-C843-49B4-9FCB-9E222CFD0814}">
   <dimension ref="A1:S149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>